<commit_message>
Links and F1 Project Update
</commit_message>
<xml_diff>
--- a/F1 2024 Preseason Testing/F1 Preseason Testing Data Collection.xlsx
+++ b/F1 2024 Preseason Testing/F1 Preseason Testing Data Collection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DataAnalystProjects\F1 2024 Preseason Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB1A1C5A-AEE7-468C-B0E8-AE20E9D56878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF71741-59CB-4EAE-B2B9-66D72734EA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5630E8B6-5D64-41B9-AED0-53F78445DC1D}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="114">
   <si>
     <t>Pos</t>
   </si>
@@ -287,6 +287,117 @@
   </si>
   <si>
     <t>Gap to Best Lap Time</t>
+  </si>
+  <si>
+    <t>Sergio Perez</t>
+  </si>
+  <si>
+    <t>Red Bull Racing</t>
+  </si>
+  <si>
+    <t>+0.758s</t>
+  </si>
+  <si>
+    <t>Lewis Hamilton</t>
+  </si>
+  <si>
+    <t>+1.145s</t>
+  </si>
+  <si>
+    <t>+1.335s</t>
+  </si>
+  <si>
+    <t>+1.440s</t>
+  </si>
+  <si>
+    <t>+1.829s</t>
+  </si>
+  <si>
+    <t>+2.108s</t>
+  </si>
+  <si>
+    <t>+2.140s</t>
+  </si>
+  <si>
+    <t>+2.306s</t>
+  </si>
+  <si>
+    <t>+2.407s</t>
+  </si>
+  <si>
+    <t>+2.657s</t>
+  </si>
+  <si>
+    <t>+3.132s</t>
+  </si>
+  <si>
+    <t>+3.794s</t>
+  </si>
+  <si>
+    <t>+3.883s</t>
+  </si>
+  <si>
+    <t>+6.690s</t>
+  </si>
+  <si>
+    <t>+7.588s</t>
+  </si>
+  <si>
+    <t>+8.153s</t>
+  </si>
+  <si>
+    <t>1:29.921s</t>
+  </si>
+  <si>
+    <t>1:30.679s</t>
+  </si>
+  <si>
+    <t>1:31.066s</t>
+  </si>
+  <si>
+    <t>1:31.256s</t>
+  </si>
+  <si>
+    <t>1:31.361s</t>
+  </si>
+  <si>
+    <t>1:31.750s</t>
+  </si>
+  <si>
+    <t>1:32.029s</t>
+  </si>
+  <si>
+    <t>1:32.061s</t>
+  </si>
+  <si>
+    <t>1:32.227s</t>
+  </si>
+  <si>
+    <t>1:32.328s</t>
+  </si>
+  <si>
+    <t>1:32.578s</t>
+  </si>
+  <si>
+    <t>1:33.053s</t>
+  </si>
+  <si>
+    <t>1:33.715s</t>
+  </si>
+  <si>
+    <t>1:33.804s</t>
+  </si>
+  <si>
+    <t>1:36.611s</t>
+  </si>
+  <si>
+    <t>1:37.509s</t>
+  </si>
+  <si>
+    <t>1:38.074s</t>
+  </si>
+  <si>
+    <t>0.000s</t>
   </si>
 </sst>
 </file>
@@ -294,7 +405,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -305,10 +416,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <color rgb="FF171F26"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -331,23 +443,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF171F26"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -369,8 +491,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5287CE3C-66D6-4CBE-8FAC-8C9AEDF89562}" name="Table1" displayName="Table1" ref="A1:J19" totalsRowShown="0">
-  <autoFilter ref="A1:J19" xr:uid="{5287CE3C-66D6-4CBE-8FAC-8C9AEDF89562}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5287CE3C-66D6-4CBE-8FAC-8C9AEDF89562}" name="Table1" displayName="Table1" ref="A1:J36" totalsRowShown="0">
+  <autoFilter ref="A1:J36" xr:uid="{5287CE3C-66D6-4CBE-8FAC-8C9AEDF89562}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{1605F3B9-F7BB-4B47-9595-74893DFEC12D}" name="Pos"/>
     <tableColumn id="2" xr3:uid="{B0699193-142E-4088-9072-AC6F1BF48846}" name="Driver"/>
@@ -723,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D4B6F7-53A3-4536-BD4D-14F09573001C}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="A1:XFD1048576"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,6 +1348,445 @@
         <v>1</v>
       </c>
     </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20">
+        <v>84</v>
+      </c>
+      <c r="G20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21">
+        <v>129</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22">
+        <v>123</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23">
+        <v>52</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24">
+        <v>88</v>
+      </c>
+      <c r="G24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25">
+        <v>54</v>
+      </c>
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26">
+        <v>96</v>
+      </c>
+      <c r="G26" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27">
+        <v>78</v>
+      </c>
+      <c r="G27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28">
+        <v>97</v>
+      </c>
+      <c r="G28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29">
+        <v>35</v>
+      </c>
+      <c r="G29" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30">
+        <v>117</v>
+      </c>
+      <c r="G30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31">
+        <v>31</v>
+      </c>
+      <c r="G31" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32">
+        <v>38</v>
+      </c>
+      <c r="G32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33">
+        <v>33</v>
+      </c>
+      <c r="G33" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34">
+        <v>93</v>
+      </c>
+      <c r="G34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" t="s">
+        <v>94</v>
+      </c>
+      <c r="F35">
+        <v>31</v>
+      </c>
+      <c r="G35" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>17</v>
+      </c>
+      <c r="B36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36">
+        <v>40</v>
+      </c>
+      <c r="G36" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1234,10 +1795,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85BF523-30CB-48A7-8E76-D50239268866}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1247,7 +1808,7 @@
     <col min="3" max="3" width="17.21875" customWidth="1"/>
     <col min="4" max="4" width="12.5546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="2" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1279,7 +1840,7 @@
       <c r="I1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1296,6 +1857,9 @@
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
       <c r="F2">
         <v>142</v>
       </c>
@@ -1306,12 +1870,12 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I19" si="0">SUBSTITUTE(D2, "s", "")</f>
+        <f t="shared" ref="I2:I20" si="0">SUBSTITUTE(D2, "s", "")</f>
         <v>1:31.344</v>
       </c>
-      <c r="J2" s="2" t="str">
-        <f t="shared" ref="J2:J19" si="1">SUBSTITUTE(SUBSTITUTE(E2,"+",""), "s", "")</f>
-        <v/>
+      <c r="J2" s="1" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(E2,"+",""), "s", "")</f>
+        <v>0.000</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1343,8 +1907,8 @@
         <f t="shared" si="0"/>
         <v>1:32.484</v>
       </c>
-      <c r="J3" s="2" t="str">
-        <f t="shared" si="1"/>
+      <c r="J3" s="1" t="str">
+        <f t="shared" ref="J2:J19" si="1">SUBSTITUTE(SUBSTITUTE(E3,"+",""), "s", "")</f>
         <v>1.140</v>
       </c>
     </row>
@@ -1377,7 +1941,7 @@
         <f t="shared" si="0"/>
         <v>1:32.584</v>
       </c>
-      <c r="J4" s="2" t="str">
+      <c r="J4" s="1" t="str">
         <f t="shared" si="1"/>
         <v>1.240</v>
       </c>
@@ -1411,7 +1975,7 @@
         <f t="shared" si="0"/>
         <v>1:32.599</v>
       </c>
-      <c r="J5" s="2" t="str">
+      <c r="J5" s="1" t="str">
         <f t="shared" si="1"/>
         <v>1.255</v>
       </c>
@@ -1445,7 +2009,7 @@
         <f t="shared" si="0"/>
         <v>1:32.805</v>
       </c>
-      <c r="J6" s="2" t="str">
+      <c r="J6" s="1" t="str">
         <f t="shared" si="1"/>
         <v>1.461</v>
       </c>
@@ -1479,7 +2043,7 @@
         <f t="shared" si="0"/>
         <v>1:33.007</v>
       </c>
-      <c r="J7" s="2" t="str">
+      <c r="J7" s="1" t="str">
         <f t="shared" si="1"/>
         <v>1.663</v>
       </c>
@@ -1513,7 +2077,7 @@
         <f t="shared" si="0"/>
         <v>1:33.247</v>
       </c>
-      <c r="J8" s="2" t="str">
+      <c r="J8" s="1" t="str">
         <f t="shared" si="1"/>
         <v>1.903</v>
       </c>
@@ -1547,7 +2111,7 @@
         <f t="shared" si="0"/>
         <v>1:33.385</v>
       </c>
-      <c r="J9" s="2" t="str">
+      <c r="J9" s="1" t="str">
         <f t="shared" si="1"/>
         <v>2.041</v>
       </c>
@@ -1581,7 +2145,7 @@
         <f t="shared" si="0"/>
         <v>1:33.658</v>
       </c>
-      <c r="J10" s="2" t="str">
+      <c r="J10" s="1" t="str">
         <f t="shared" si="1"/>
         <v>2.314</v>
       </c>
@@ -1615,7 +2179,7 @@
         <f t="shared" si="0"/>
         <v>1:33.871</v>
       </c>
-      <c r="J11" s="2" t="str">
+      <c r="J11" s="1" t="str">
         <f t="shared" si="1"/>
         <v>2.527</v>
       </c>
@@ -1649,7 +2213,7 @@
         <f t="shared" si="0"/>
         <v>1:33.882</v>
       </c>
-      <c r="J12" s="2" t="str">
+      <c r="J12" s="1" t="str">
         <f t="shared" si="1"/>
         <v>2.538</v>
       </c>
@@ -1683,7 +2247,7 @@
         <f t="shared" si="0"/>
         <v>1:34.109</v>
       </c>
-      <c r="J13" s="2" t="str">
+      <c r="J13" s="1" t="str">
         <f t="shared" si="1"/>
         <v>2.765</v>
       </c>
@@ -1717,7 +2281,7 @@
         <f t="shared" si="0"/>
         <v>1:34.136</v>
       </c>
-      <c r="J14" s="2" t="str">
+      <c r="J14" s="1" t="str">
         <f t="shared" si="1"/>
         <v>2.792</v>
       </c>
@@ -1751,7 +2315,7 @@
         <f t="shared" si="0"/>
         <v>1:34.431</v>
       </c>
-      <c r="J15" s="2" t="str">
+      <c r="J15" s="1" t="str">
         <f t="shared" si="1"/>
         <v>3.087</v>
       </c>
@@ -1785,7 +2349,7 @@
         <f t="shared" si="0"/>
         <v>1:34.587</v>
       </c>
-      <c r="J16" s="2" t="str">
+      <c r="J16" s="1" t="str">
         <f t="shared" si="1"/>
         <v>3.243</v>
       </c>
@@ -1819,7 +2383,7 @@
         <f t="shared" si="0"/>
         <v>1:34.677</v>
       </c>
-      <c r="J17" s="2" t="str">
+      <c r="J17" s="1" t="str">
         <f t="shared" si="1"/>
         <v>3.333</v>
       </c>
@@ -1853,7 +2417,7 @@
         <f t="shared" si="0"/>
         <v>1:35.692</v>
       </c>
-      <c r="J18" s="2" t="str">
+      <c r="J18" s="1" t="str">
         <f t="shared" si="1"/>
         <v>4.348</v>
       </c>
@@ -1887,9 +2451,587 @@
         <f t="shared" si="0"/>
         <v>1:35.906</v>
       </c>
-      <c r="J19" s="2" t="str">
+      <c r="J19" s="1" t="str">
         <f t="shared" si="1"/>
         <v>4.562</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20">
+        <v>84</v>
+      </c>
+      <c r="G20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>1:29.921</v>
+      </c>
+      <c r="J20" s="1" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(E20,"+",""), "s", "")</f>
+        <v>0.000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21">
+        <v>129</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21" s="2" t="str">
+        <f t="shared" ref="I21:I36" si="2">SUBSTITUTE(D21, "s", "")</f>
+        <v>1:30.679</v>
+      </c>
+      <c r="J21" s="1" t="str">
+        <f t="shared" ref="J20:J36" si="3">SUBSTITUTE(SUBSTITUTE(E21,"+",""), "s", "")</f>
+        <v>0.758</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22">
+        <v>123</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:31.066</v>
+      </c>
+      <c r="J22" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>1.145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23">
+        <v>52</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:31.256</v>
+      </c>
+      <c r="J23" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>1.335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24">
+        <v>88</v>
+      </c>
+      <c r="G24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:31.361</v>
+      </c>
+      <c r="J24" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>1.440</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25">
+        <v>54</v>
+      </c>
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:31.750</v>
+      </c>
+      <c r="J25" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>1.829</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26">
+        <v>96</v>
+      </c>
+      <c r="G26" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:32.029</v>
+      </c>
+      <c r="J26" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>2.108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27">
+        <v>78</v>
+      </c>
+      <c r="G27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:32.061</v>
+      </c>
+      <c r="J27" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>2.140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28">
+        <v>97</v>
+      </c>
+      <c r="G28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:32.227</v>
+      </c>
+      <c r="J28" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>2.306</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29">
+        <v>35</v>
+      </c>
+      <c r="G29" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:32.328</v>
+      </c>
+      <c r="J29" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>2.407</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30">
+        <v>117</v>
+      </c>
+      <c r="G30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:32.578</v>
+      </c>
+      <c r="J30" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>2.657</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31">
+        <v>31</v>
+      </c>
+      <c r="G31" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:33.053</v>
+      </c>
+      <c r="J31" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>3.132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32">
+        <v>38</v>
+      </c>
+      <c r="G32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:33.715</v>
+      </c>
+      <c r="J32" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>3.794</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33">
+        <v>33</v>
+      </c>
+      <c r="G33" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:33.804</v>
+      </c>
+      <c r="J33" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>3.883</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34">
+        <v>93</v>
+      </c>
+      <c r="G34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:36.611</v>
+      </c>
+      <c r="J34" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>6.690</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" t="s">
+        <v>94</v>
+      </c>
+      <c r="F35">
+        <v>31</v>
+      </c>
+      <c r="G35" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:37.509</v>
+      </c>
+      <c r="J35" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>7.588</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>17</v>
+      </c>
+      <c r="B36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36">
+        <v>40</v>
+      </c>
+      <c r="G36" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1:38.074</v>
+      </c>
+      <c r="J36" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>8.153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data Updates and F1 Preseason
</commit_message>
<xml_diff>
--- a/F1 2024 Preseason Testing/F1 Preseason Testing Data Collection.xlsx
+++ b/F1 2024 Preseason Testing/F1 Preseason Testing Data Collection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DataAnalystProjects\F1 2024 Preseason Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF71741-59CB-4EAE-B2B9-66D72734EA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36609F0-0B40-49FF-AD95-755DAFD2A9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5630E8B6-5D64-41B9-AED0-53F78445DC1D}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="151">
   <si>
     <t>Pos</t>
   </si>
@@ -398,6 +398,117 @@
   </si>
   <si>
     <t>0.000s</t>
+  </si>
+  <si>
+    <t>+0.046s</t>
+  </si>
+  <si>
+    <t>+0.325s</t>
+  </si>
+  <si>
+    <t>+0.433s</t>
+  </si>
+  <si>
+    <t>+0.453s</t>
+  </si>
+  <si>
+    <t>+0.662s</t>
+  </si>
+  <si>
+    <t>+0.708s</t>
+  </si>
+  <si>
+    <t>+0.837s</t>
+  </si>
+  <si>
+    <t>+0.925s</t>
+  </si>
+  <si>
+    <t>+1.161s</t>
+  </si>
+  <si>
+    <t>+1.364s</t>
+  </si>
+  <si>
+    <t>+1.677s</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>+1.716s</t>
+  </si>
+  <si>
+    <t>+1.786s</t>
+  </si>
+  <si>
+    <t>+1.827s</t>
+  </si>
+  <si>
+    <t>+2.731s</t>
+  </si>
+  <si>
+    <t>+2.757s</t>
+  </si>
+  <si>
+    <t>+3.206s</t>
+  </si>
+  <si>
+    <t>+6.693s</t>
+  </si>
+  <si>
+    <t>1:30.322s</t>
+  </si>
+  <si>
+    <t>1:30.368s</t>
+  </si>
+  <si>
+    <t>1:30.647s</t>
+  </si>
+  <si>
+    <t>1:30.755s</t>
+  </si>
+  <si>
+    <t>1:30.775s</t>
+  </si>
+  <si>
+    <t>1:30.984s</t>
+  </si>
+  <si>
+    <t>1:31.030s</t>
+  </si>
+  <si>
+    <t>1:31.159s</t>
+  </si>
+  <si>
+    <t>1:31.247s</t>
+  </si>
+  <si>
+    <t>1:31.483s</t>
+  </si>
+  <si>
+    <t>1:31.686s</t>
+  </si>
+  <si>
+    <t>1:31.999s</t>
+  </si>
+  <si>
+    <t>1:32.038s</t>
+  </si>
+  <si>
+    <t>1:32.108s</t>
+  </si>
+  <si>
+    <t>1:32.149s</t>
+  </si>
+  <si>
+    <t>1:33.079s</t>
+  </si>
+  <si>
+    <t>1:33.528s</t>
+  </si>
+  <si>
+    <t>1:37.015s</t>
   </si>
 </sst>
 </file>
@@ -456,12 +567,6 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF171F26"/>
         <name val="Aptos Display"/>
@@ -470,6 +575,12 @@
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -491,21 +602,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5287CE3C-66D6-4CBE-8FAC-8C9AEDF89562}" name="Table1" displayName="Table1" ref="A1:J36" totalsRowShown="0">
-  <autoFilter ref="A1:J36" xr:uid="{5287CE3C-66D6-4CBE-8FAC-8C9AEDF89562}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5287CE3C-66D6-4CBE-8FAC-8C9AEDF89562}" name="Table1" displayName="Table1" ref="A1:J55" totalsRowShown="0">
+  <autoFilter ref="A1:J55" xr:uid="{5287CE3C-66D6-4CBE-8FAC-8C9AEDF89562}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{1605F3B9-F7BB-4B47-9595-74893DFEC12D}" name="Pos"/>
     <tableColumn id="2" xr3:uid="{B0699193-142E-4088-9072-AC6F1BF48846}" name="Driver"/>
     <tableColumn id="3" xr3:uid="{009811E6-BC1C-462E-B859-C279CF81CBB6}" name="Team"/>
-    <tableColumn id="4" xr3:uid="{57D4AD65-2EC3-4640-91F5-BE832D592422}" name="Time" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{57D4AD65-2EC3-4640-91F5-BE832D592422}" name="Time" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{8A29713F-6989-4D54-B260-CD548B059286}" name="Gap"/>
     <tableColumn id="6" xr3:uid="{365C61E4-18D0-4B6F-B11C-79AB3F42AE04}" name="Laps"/>
     <tableColumn id="7" xr3:uid="{C3262CC7-6DEC-4497-B05A-A21C0F6AE33A}" name="Tyres"/>
     <tableColumn id="8" xr3:uid="{90ACD433-CF4C-4370-B351-0D97CA1A2189}" name="Day"/>
-    <tableColumn id="9" xr3:uid="{BBED0197-BB85-4165-A816-02E8E2B7B387}" name="Best Lap Time" dataDxfId="1">
+    <tableColumn id="9" xr3:uid="{BBED0197-BB85-4165-A816-02E8E2B7B387}" name="Best Lap Time" dataDxfId="2">
       <calculatedColumnFormula>SUBSTITUTE(D2, "s", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{7B18573B-AA06-4662-B8EE-F205A25E907B}" name="Gap to Best Lap Time" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{7B18573B-AA06-4662-B8EE-F205A25E907B}" name="Gap to Best Lap Time" dataDxfId="1">
       <calculatedColumnFormula>SUBSTITUTE(SUBSTITUTE(E2,"+",""), "s", "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -845,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D4B6F7-53A3-4536-BD4D-14F09573001C}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H55" sqref="A2:H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1787,6 +1898,497 @@
         <v>2</v>
       </c>
     </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F37">
+        <v>74</v>
+      </c>
+      <c r="G37" t="s">
+        <v>62</v>
+      </c>
+      <c r="H37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" t="s">
+        <v>114</v>
+      </c>
+      <c r="F38">
+        <v>67</v>
+      </c>
+      <c r="G38" t="s">
+        <v>62</v>
+      </c>
+      <c r="H38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39">
+        <v>85</v>
+      </c>
+      <c r="G39" t="s">
+        <v>62</v>
+      </c>
+      <c r="H39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E40" t="s">
+        <v>116</v>
+      </c>
+      <c r="F40">
+        <v>66</v>
+      </c>
+      <c r="G40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" t="s">
+        <v>117</v>
+      </c>
+      <c r="F41">
+        <v>53</v>
+      </c>
+      <c r="G41" t="s">
+        <v>62</v>
+      </c>
+      <c r="H41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" t="s">
+        <v>118</v>
+      </c>
+      <c r="F42">
+        <v>121</v>
+      </c>
+      <c r="G42" t="s">
+        <v>62</v>
+      </c>
+      <c r="H42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43" t="s">
+        <v>119</v>
+      </c>
+      <c r="F43">
+        <v>91</v>
+      </c>
+      <c r="G43" t="s">
+        <v>10</v>
+      </c>
+      <c r="H43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E44" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44">
+        <v>75</v>
+      </c>
+      <c r="G44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E45" t="s">
+        <v>121</v>
+      </c>
+      <c r="F45">
+        <v>71</v>
+      </c>
+      <c r="G45" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E46" t="s">
+        <v>122</v>
+      </c>
+      <c r="F46">
+        <v>53</v>
+      </c>
+      <c r="G46" t="s">
+        <v>10</v>
+      </c>
+      <c r="H46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E47" t="s">
+        <v>123</v>
+      </c>
+      <c r="F47">
+        <v>89</v>
+      </c>
+      <c r="G47" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E48" t="s">
+        <v>124</v>
+      </c>
+      <c r="F48">
+        <v>49</v>
+      </c>
+      <c r="G48" t="s">
+        <v>125</v>
+      </c>
+      <c r="H48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>13</v>
+      </c>
+      <c r="B49" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E49" t="s">
+        <v>126</v>
+      </c>
+      <c r="F49">
+        <v>46</v>
+      </c>
+      <c r="G49" t="s">
+        <v>10</v>
+      </c>
+      <c r="H49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E50" t="s">
+        <v>127</v>
+      </c>
+      <c r="F50">
+        <v>20</v>
+      </c>
+      <c r="G50" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>15</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E51" t="s">
+        <v>128</v>
+      </c>
+      <c r="F51">
+        <v>47</v>
+      </c>
+      <c r="G51" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>16</v>
+      </c>
+      <c r="B52" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E52" t="s">
+        <v>129</v>
+      </c>
+      <c r="F52">
+        <v>80</v>
+      </c>
+      <c r="G52" t="s">
+        <v>10</v>
+      </c>
+      <c r="H52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>17</v>
+      </c>
+      <c r="B53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E53" t="s">
+        <v>130</v>
+      </c>
+      <c r="F53">
+        <v>55</v>
+      </c>
+      <c r="G53" t="s">
+        <v>10</v>
+      </c>
+      <c r="H53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>18</v>
+      </c>
+      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" t="s">
+        <v>41</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E54" t="s">
+        <v>131</v>
+      </c>
+      <c r="F54">
+        <v>28</v>
+      </c>
+      <c r="G54" t="s">
+        <v>10</v>
+      </c>
+      <c r="H54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>19</v>
+      </c>
+      <c r="B55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E55" t="s">
+        <v>132</v>
+      </c>
+      <c r="F55">
+        <v>70</v>
+      </c>
+      <c r="G55" t="s">
+        <v>66</v>
+      </c>
+      <c r="H55">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1795,10 +2397,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85BF523-30CB-48A7-8E76-D50239268866}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1908,7 +2510,7 @@
         <v>1:32.484</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f t="shared" ref="J2:J19" si="1">SUBSTITUTE(SUBSTITUTE(E3,"+",""), "s", "")</f>
+        <f t="shared" ref="J3:J19" si="1">SUBSTITUTE(SUBSTITUTE(E3,"+",""), "s", "")</f>
         <v>1.140</v>
       </c>
     </row>
@@ -2520,7 +3122,7 @@
         <v>1:30.679</v>
       </c>
       <c r="J21" s="1" t="str">
-        <f t="shared" ref="J20:J36" si="3">SUBSTITUTE(SUBSTITUTE(E21,"+",""), "s", "")</f>
+        <f t="shared" ref="J21:J36" si="3">SUBSTITUTE(SUBSTITUTE(E21,"+",""), "s", "")</f>
         <v>0.758</v>
       </c>
     </row>
@@ -3032,6 +3634,652 @@
       <c r="J36" s="1" t="str">
         <f t="shared" si="3"/>
         <v>8.153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" t="s">
+        <v>113</v>
+      </c>
+      <c r="F37">
+        <v>74</v>
+      </c>
+      <c r="G37" t="s">
+        <v>62</v>
+      </c>
+      <c r="H37">
+        <v>3</v>
+      </c>
+      <c r="I37" s="2" t="str">
+        <f t="shared" ref="I37:I55" si="4">SUBSTITUTE(D37, "s", "")</f>
+        <v>1:30.322</v>
+      </c>
+      <c r="J37" s="1" t="str">
+        <f t="shared" ref="J37:J55" si="5">SUBSTITUTE(SUBSTITUTE(E37,"+",""), "s", "")</f>
+        <v>0.000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" t="s">
+        <v>114</v>
+      </c>
+      <c r="F38">
+        <v>67</v>
+      </c>
+      <c r="G38" t="s">
+        <v>62</v>
+      </c>
+      <c r="H38">
+        <v>3</v>
+      </c>
+      <c r="I38" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:30.368</v>
+      </c>
+      <c r="J38" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>0.046</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39">
+        <v>85</v>
+      </c>
+      <c r="G39" t="s">
+        <v>62</v>
+      </c>
+      <c r="H39">
+        <v>3</v>
+      </c>
+      <c r="I39" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:30.647</v>
+      </c>
+      <c r="J39" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>0.325</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E40" t="s">
+        <v>116</v>
+      </c>
+      <c r="F40">
+        <v>66</v>
+      </c>
+      <c r="G40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:30.755</v>
+      </c>
+      <c r="J40" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>0.433</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" t="s">
+        <v>117</v>
+      </c>
+      <c r="F41">
+        <v>53</v>
+      </c>
+      <c r="G41" t="s">
+        <v>62</v>
+      </c>
+      <c r="H41">
+        <v>3</v>
+      </c>
+      <c r="I41" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:30.775</v>
+      </c>
+      <c r="J41" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>0.453</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" t="s">
+        <v>118</v>
+      </c>
+      <c r="F42">
+        <v>121</v>
+      </c>
+      <c r="G42" t="s">
+        <v>62</v>
+      </c>
+      <c r="H42">
+        <v>3</v>
+      </c>
+      <c r="I42" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:30.984</v>
+      </c>
+      <c r="J42" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>0.662</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43" t="s">
+        <v>119</v>
+      </c>
+      <c r="F43">
+        <v>91</v>
+      </c>
+      <c r="G43" t="s">
+        <v>10</v>
+      </c>
+      <c r="H43">
+        <v>3</v>
+      </c>
+      <c r="I43" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:31.030</v>
+      </c>
+      <c r="J43" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>0.708</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E44" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44">
+        <v>75</v>
+      </c>
+      <c r="G44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44">
+        <v>3</v>
+      </c>
+      <c r="I44" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:31.159</v>
+      </c>
+      <c r="J44" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>0.837</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E45" t="s">
+        <v>121</v>
+      </c>
+      <c r="F45">
+        <v>71</v>
+      </c>
+      <c r="G45" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45">
+        <v>3</v>
+      </c>
+      <c r="I45" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:31.247</v>
+      </c>
+      <c r="J45" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>0.925</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E46" t="s">
+        <v>122</v>
+      </c>
+      <c r="F46">
+        <v>53</v>
+      </c>
+      <c r="G46" t="s">
+        <v>10</v>
+      </c>
+      <c r="H46">
+        <v>3</v>
+      </c>
+      <c r="I46" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:31.483</v>
+      </c>
+      <c r="J46" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1.161</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E47" t="s">
+        <v>123</v>
+      </c>
+      <c r="F47">
+        <v>89</v>
+      </c>
+      <c r="G47" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47">
+        <v>3</v>
+      </c>
+      <c r="I47" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:31.686</v>
+      </c>
+      <c r="J47" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1.364</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E48" t="s">
+        <v>124</v>
+      </c>
+      <c r="F48">
+        <v>49</v>
+      </c>
+      <c r="G48" t="s">
+        <v>125</v>
+      </c>
+      <c r="H48">
+        <v>3</v>
+      </c>
+      <c r="I48" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:31.999</v>
+      </c>
+      <c r="J48" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1.677</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>13</v>
+      </c>
+      <c r="B49" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E49" t="s">
+        <v>126</v>
+      </c>
+      <c r="F49">
+        <v>46</v>
+      </c>
+      <c r="G49" t="s">
+        <v>10</v>
+      </c>
+      <c r="H49">
+        <v>3</v>
+      </c>
+      <c r="I49" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:32.038</v>
+      </c>
+      <c r="J49" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1.716</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E50" t="s">
+        <v>127</v>
+      </c>
+      <c r="F50">
+        <v>20</v>
+      </c>
+      <c r="G50" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50">
+        <v>3</v>
+      </c>
+      <c r="I50" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:32.108</v>
+      </c>
+      <c r="J50" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1.786</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>15</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E51" t="s">
+        <v>128</v>
+      </c>
+      <c r="F51">
+        <v>47</v>
+      </c>
+      <c r="G51" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51">
+        <v>3</v>
+      </c>
+      <c r="I51" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:32.149</v>
+      </c>
+      <c r="J51" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1.827</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>16</v>
+      </c>
+      <c r="B52" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E52" t="s">
+        <v>129</v>
+      </c>
+      <c r="F52">
+        <v>80</v>
+      </c>
+      <c r="G52" t="s">
+        <v>10</v>
+      </c>
+      <c r="H52">
+        <v>3</v>
+      </c>
+      <c r="I52" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:33.053</v>
+      </c>
+      <c r="J52" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>2.731</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>17</v>
+      </c>
+      <c r="B53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E53" t="s">
+        <v>130</v>
+      </c>
+      <c r="F53">
+        <v>55</v>
+      </c>
+      <c r="G53" t="s">
+        <v>10</v>
+      </c>
+      <c r="H53">
+        <v>3</v>
+      </c>
+      <c r="I53" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:33.079</v>
+      </c>
+      <c r="J53" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>2.757</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>18</v>
+      </c>
+      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" t="s">
+        <v>41</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E54" t="s">
+        <v>131</v>
+      </c>
+      <c r="F54">
+        <v>28</v>
+      </c>
+      <c r="G54" t="s">
+        <v>10</v>
+      </c>
+      <c r="H54">
+        <v>3</v>
+      </c>
+      <c r="I54" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:33.528</v>
+      </c>
+      <c r="J54" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>3.206</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>19</v>
+      </c>
+      <c r="B55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E55" t="s">
+        <v>132</v>
+      </c>
+      <c r="F55">
+        <v>70</v>
+      </c>
+      <c r="G55" t="s">
+        <v>66</v>
+      </c>
+      <c r="H55">
+        <v>3</v>
+      </c>
+      <c r="I55" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>1:37.015</v>
+      </c>
+      <c r="J55" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>6.693</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
F1, Conditional, Tableau, SQL Updates
</commit_message>
<xml_diff>
--- a/F1 2024 Preseason Testing/F1 Preseason Testing Data Collection.xlsx
+++ b/F1 2024 Preseason Testing/F1 Preseason Testing Data Collection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DataAnalystProjects\F1 2024 Preseason Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36609F0-0B40-49FF-AD95-755DAFD2A9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28203E7-D269-4A63-A41F-D1E568CC913A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5630E8B6-5D64-41B9-AED0-53F78445DC1D}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="152">
   <si>
     <t>Pos</t>
   </si>
@@ -509,14 +509,18 @@
   </si>
   <si>
     <t>1:37.015s</t>
+  </si>
+  <si>
+    <t>Position</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="mm:ss.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -554,18 +558,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="mm:ss.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF171F26"/>
@@ -575,12 +586,6 @@
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -605,15 +610,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5287CE3C-66D6-4CBE-8FAC-8C9AEDF89562}" name="Table1" displayName="Table1" ref="A1:J55" totalsRowShown="0">
   <autoFilter ref="A1:J55" xr:uid="{5287CE3C-66D6-4CBE-8FAC-8C9AEDF89562}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{1605F3B9-F7BB-4B47-9595-74893DFEC12D}" name="Pos"/>
+    <tableColumn id="1" xr3:uid="{1605F3B9-F7BB-4B47-9595-74893DFEC12D}" name="Position"/>
     <tableColumn id="2" xr3:uid="{B0699193-142E-4088-9072-AC6F1BF48846}" name="Driver"/>
     <tableColumn id="3" xr3:uid="{009811E6-BC1C-462E-B859-C279CF81CBB6}" name="Team"/>
-    <tableColumn id="4" xr3:uid="{57D4AD65-2EC3-4640-91F5-BE832D592422}" name="Time" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{57D4AD65-2EC3-4640-91F5-BE832D592422}" name="Time" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{8A29713F-6989-4D54-B260-CD548B059286}" name="Gap"/>
     <tableColumn id="6" xr3:uid="{365C61E4-18D0-4B6F-B11C-79AB3F42AE04}" name="Laps"/>
     <tableColumn id="7" xr3:uid="{C3262CC7-6DEC-4497-B05A-A21C0F6AE33A}" name="Tyres"/>
     <tableColumn id="8" xr3:uid="{90ACD433-CF4C-4370-B351-0D97CA1A2189}" name="Day"/>
-    <tableColumn id="9" xr3:uid="{BBED0197-BB85-4165-A816-02E8E2B7B387}" name="Best Lap Time" dataDxfId="2">
+    <tableColumn id="9" xr3:uid="{BBED0197-BB85-4165-A816-02E8E2B7B387}" name="Best Lap Time" dataDxfId="0">
       <calculatedColumnFormula>SUBSTITUTE(D2, "s", "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{7B18573B-AA06-4662-B8EE-F205A25E907B}" name="Gap to Best Lap Time" dataDxfId="1">
@@ -2400,7 +2405,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2409,14 +2414,14 @@
     <col min="2" max="2" width="21.88671875" customWidth="1"/>
     <col min="3" max="3" width="17.21875" customWidth="1"/>
     <col min="4" max="4" width="12.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15" style="4" customWidth="1"/>
     <col min="10" max="10" width="20.6640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2471,7 +2476,7 @@
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="str">
+      <c r="I2" s="4" t="str">
         <f t="shared" ref="I2:I20" si="0">SUBSTITUTE(D2, "s", "")</f>
         <v>1:31.344</v>
       </c>
@@ -2505,7 +2510,7 @@
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" s="2" t="str">
+      <c r="I3" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:32.484</v>
       </c>
@@ -2539,7 +2544,7 @@
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" s="2" t="str">
+      <c r="I4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:32.584</v>
       </c>
@@ -2573,7 +2578,7 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="I5" s="2" t="str">
+      <c r="I5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:32.599</v>
       </c>
@@ -2607,7 +2612,7 @@
       <c r="H6">
         <v>1</v>
       </c>
-      <c r="I6" s="2" t="str">
+      <c r="I6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:32.805</v>
       </c>
@@ -2641,7 +2646,7 @@
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="I7" s="2" t="str">
+      <c r="I7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:33.007</v>
       </c>
@@ -2675,7 +2680,7 @@
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8" s="2" t="str">
+      <c r="I8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:33.247</v>
       </c>
@@ -2709,7 +2714,7 @@
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" s="2" t="str">
+      <c r="I9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:33.385</v>
       </c>
@@ -2743,7 +2748,7 @@
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10" s="2" t="str">
+      <c r="I10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:33.658</v>
       </c>
@@ -2777,7 +2782,7 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11" s="2" t="str">
+      <c r="I11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:33.871</v>
       </c>
@@ -2811,7 +2816,7 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12" s="2" t="str">
+      <c r="I12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:33.882</v>
       </c>
@@ -2845,7 +2850,7 @@
       <c r="H13">
         <v>1</v>
       </c>
-      <c r="I13" s="2" t="str">
+      <c r="I13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:34.109</v>
       </c>
@@ -2879,7 +2884,7 @@
       <c r="H14">
         <v>1</v>
       </c>
-      <c r="I14" s="2" t="str">
+      <c r="I14" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:34.136</v>
       </c>
@@ -2913,7 +2918,7 @@
       <c r="H15">
         <v>1</v>
       </c>
-      <c r="I15" s="2" t="str">
+      <c r="I15" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:34.431</v>
       </c>
@@ -2947,7 +2952,7 @@
       <c r="H16">
         <v>1</v>
       </c>
-      <c r="I16" s="2" t="str">
+      <c r="I16" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:34.587</v>
       </c>
@@ -2981,7 +2986,7 @@
       <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17" s="2" t="str">
+      <c r="I17" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:34.677</v>
       </c>
@@ -3015,7 +3020,7 @@
       <c r="H18">
         <v>1</v>
       </c>
-      <c r="I18" s="2" t="str">
+      <c r="I18" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:35.692</v>
       </c>
@@ -3049,7 +3054,7 @@
       <c r="H19">
         <v>1</v>
       </c>
-      <c r="I19" s="2" t="str">
+      <c r="I19" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:35.906</v>
       </c>
@@ -3083,7 +3088,7 @@
       <c r="H20">
         <v>2</v>
       </c>
-      <c r="I20" s="2" t="str">
+      <c r="I20" s="4" t="str">
         <f t="shared" si="0"/>
         <v>1:29.921</v>
       </c>
@@ -3117,7 +3122,7 @@
       <c r="H21">
         <v>2</v>
       </c>
-      <c r="I21" s="2" t="str">
+      <c r="I21" s="4" t="str">
         <f t="shared" ref="I21:I36" si="2">SUBSTITUTE(D21, "s", "")</f>
         <v>1:30.679</v>
       </c>
@@ -3151,7 +3156,7 @@
       <c r="H22">
         <v>2</v>
       </c>
-      <c r="I22" s="2" t="str">
+      <c r="I22" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:31.066</v>
       </c>
@@ -3185,7 +3190,7 @@
       <c r="H23">
         <v>2</v>
       </c>
-      <c r="I23" s="2" t="str">
+      <c r="I23" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:31.256</v>
       </c>
@@ -3219,7 +3224,7 @@
       <c r="H24">
         <v>2</v>
       </c>
-      <c r="I24" s="2" t="str">
+      <c r="I24" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:31.361</v>
       </c>
@@ -3253,7 +3258,7 @@
       <c r="H25">
         <v>2</v>
       </c>
-      <c r="I25" s="2" t="str">
+      <c r="I25" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:31.750</v>
       </c>
@@ -3287,7 +3292,7 @@
       <c r="H26">
         <v>2</v>
       </c>
-      <c r="I26" s="2" t="str">
+      <c r="I26" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:32.029</v>
       </c>
@@ -3321,7 +3326,7 @@
       <c r="H27">
         <v>2</v>
       </c>
-      <c r="I27" s="2" t="str">
+      <c r="I27" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:32.061</v>
       </c>
@@ -3355,7 +3360,7 @@
       <c r="H28">
         <v>2</v>
       </c>
-      <c r="I28" s="2" t="str">
+      <c r="I28" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:32.227</v>
       </c>
@@ -3389,7 +3394,7 @@
       <c r="H29">
         <v>2</v>
       </c>
-      <c r="I29" s="2" t="str">
+      <c r="I29" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:32.328</v>
       </c>
@@ -3423,7 +3428,7 @@
       <c r="H30">
         <v>2</v>
       </c>
-      <c r="I30" s="2" t="str">
+      <c r="I30" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:32.578</v>
       </c>
@@ -3457,7 +3462,7 @@
       <c r="H31">
         <v>2</v>
       </c>
-      <c r="I31" s="2" t="str">
+      <c r="I31" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:33.053</v>
       </c>
@@ -3491,7 +3496,7 @@
       <c r="H32">
         <v>2</v>
       </c>
-      <c r="I32" s="2" t="str">
+      <c r="I32" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:33.715</v>
       </c>
@@ -3525,7 +3530,7 @@
       <c r="H33">
         <v>2</v>
       </c>
-      <c r="I33" s="2" t="str">
+      <c r="I33" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:33.804</v>
       </c>
@@ -3559,7 +3564,7 @@
       <c r="H34">
         <v>2</v>
       </c>
-      <c r="I34" s="2" t="str">
+      <c r="I34" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:36.611</v>
       </c>
@@ -3593,7 +3598,7 @@
       <c r="H35">
         <v>2</v>
       </c>
-      <c r="I35" s="2" t="str">
+      <c r="I35" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:37.509</v>
       </c>
@@ -3627,7 +3632,7 @@
       <c r="H36">
         <v>2</v>
       </c>
-      <c r="I36" s="2" t="str">
+      <c r="I36" s="4" t="str">
         <f t="shared" si="2"/>
         <v>1:38.074</v>
       </c>
@@ -3661,7 +3666,7 @@
       <c r="H37">
         <v>3</v>
       </c>
-      <c r="I37" s="2" t="str">
+      <c r="I37" s="4" t="str">
         <f t="shared" ref="I37:I55" si="4">SUBSTITUTE(D37, "s", "")</f>
         <v>1:30.322</v>
       </c>
@@ -3695,7 +3700,7 @@
       <c r="H38">
         <v>3</v>
       </c>
-      <c r="I38" s="2" t="str">
+      <c r="I38" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:30.368</v>
       </c>
@@ -3729,7 +3734,7 @@
       <c r="H39">
         <v>3</v>
       </c>
-      <c r="I39" s="2" t="str">
+      <c r="I39" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:30.647</v>
       </c>
@@ -3763,7 +3768,7 @@
       <c r="H40">
         <v>3</v>
       </c>
-      <c r="I40" s="2" t="str">
+      <c r="I40" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:30.755</v>
       </c>
@@ -3797,7 +3802,7 @@
       <c r="H41">
         <v>3</v>
       </c>
-      <c r="I41" s="2" t="str">
+      <c r="I41" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:30.775</v>
       </c>
@@ -3831,7 +3836,7 @@
       <c r="H42">
         <v>3</v>
       </c>
-      <c r="I42" s="2" t="str">
+      <c r="I42" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:30.984</v>
       </c>
@@ -3865,7 +3870,7 @@
       <c r="H43">
         <v>3</v>
       </c>
-      <c r="I43" s="2" t="str">
+      <c r="I43" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:31.030</v>
       </c>
@@ -3899,7 +3904,7 @@
       <c r="H44">
         <v>3</v>
       </c>
-      <c r="I44" s="2" t="str">
+      <c r="I44" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:31.159</v>
       </c>
@@ -3933,7 +3938,7 @@
       <c r="H45">
         <v>3</v>
       </c>
-      <c r="I45" s="2" t="str">
+      <c r="I45" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:31.247</v>
       </c>
@@ -3967,7 +3972,7 @@
       <c r="H46">
         <v>3</v>
       </c>
-      <c r="I46" s="2" t="str">
+      <c r="I46" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:31.483</v>
       </c>
@@ -4001,7 +4006,7 @@
       <c r="H47">
         <v>3</v>
       </c>
-      <c r="I47" s="2" t="str">
+      <c r="I47" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:31.686</v>
       </c>
@@ -4035,7 +4040,7 @@
       <c r="H48">
         <v>3</v>
       </c>
-      <c r="I48" s="2" t="str">
+      <c r="I48" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:31.999</v>
       </c>
@@ -4069,7 +4074,7 @@
       <c r="H49">
         <v>3</v>
       </c>
-      <c r="I49" s="2" t="str">
+      <c r="I49" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:32.038</v>
       </c>
@@ -4103,7 +4108,7 @@
       <c r="H50">
         <v>3</v>
       </c>
-      <c r="I50" s="2" t="str">
+      <c r="I50" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:32.108</v>
       </c>
@@ -4137,7 +4142,7 @@
       <c r="H51">
         <v>3</v>
       </c>
-      <c r="I51" s="2" t="str">
+      <c r="I51" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:32.149</v>
       </c>
@@ -4171,7 +4176,7 @@
       <c r="H52">
         <v>3</v>
       </c>
-      <c r="I52" s="2" t="str">
+      <c r="I52" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:33.053</v>
       </c>
@@ -4205,7 +4210,7 @@
       <c r="H53">
         <v>3</v>
       </c>
-      <c r="I53" s="2" t="str">
+      <c r="I53" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:33.079</v>
       </c>
@@ -4239,7 +4244,7 @@
       <c r="H54">
         <v>3</v>
       </c>
-      <c r="I54" s="2" t="str">
+      <c r="I54" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:33.528</v>
       </c>
@@ -4273,7 +4278,7 @@
       <c r="H55">
         <v>3</v>
       </c>
-      <c r="I55" s="2" t="str">
+      <c r="I55" s="4" t="str">
         <f t="shared" si="4"/>
         <v>1:37.015</v>
       </c>

</xml_diff>

<commit_message>
F1 Preseason Testing Project Complete
</commit_message>
<xml_diff>
--- a/F1 2024 Preseason Testing/F1 Preseason Testing Data Collection.xlsx
+++ b/F1 2024 Preseason Testing/F1 Preseason Testing Data Collection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DataAnalystProjects\F1 2024 Preseason Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67ACBFC6-84A1-4555-8ED5-18F7AD20B3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7635064F-A154-4B34-B7DA-9C222EC539D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5630E8B6-5D64-41B9-AED0-53F78445DC1D}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="153">
   <si>
     <t>Pos</t>
   </si>
@@ -512,6 +512,9 @@
   </si>
   <si>
     <t>Position</t>
+  </si>
+  <si>
+    <t>Best Lap Times</t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -607,22 +613,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5287CE3C-66D6-4CBE-8FAC-8C9AEDF89562}" name="Table1" displayName="Table1" ref="A1:J55" totalsRowShown="0">
-  <autoFilter ref="A1:J55" xr:uid="{5287CE3C-66D6-4CBE-8FAC-8C9AEDF89562}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5287CE3C-66D6-4CBE-8FAC-8C9AEDF89562}" name="Table1" displayName="Table1" ref="A1:K55" totalsRowShown="0">
+  <autoFilter ref="A1:K55" xr:uid="{5287CE3C-66D6-4CBE-8FAC-8C9AEDF89562}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{1605F3B9-F7BB-4B47-9595-74893DFEC12D}" name="Position"/>
     <tableColumn id="2" xr3:uid="{B0699193-142E-4088-9072-AC6F1BF48846}" name="Driver"/>
     <tableColumn id="3" xr3:uid="{009811E6-BC1C-462E-B859-C279CF81CBB6}" name="Team"/>
-    <tableColumn id="4" xr3:uid="{57D4AD65-2EC3-4640-91F5-BE832D592422}" name="Time" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{57D4AD65-2EC3-4640-91F5-BE832D592422}" name="Time" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{8A29713F-6989-4D54-B260-CD548B059286}" name="Gap"/>
     <tableColumn id="6" xr3:uid="{365C61E4-18D0-4B6F-B11C-79AB3F42AE04}" name="Laps"/>
     <tableColumn id="7" xr3:uid="{C3262CC7-6DEC-4497-B05A-A21C0F6AE33A}" name="Tyres"/>
     <tableColumn id="8" xr3:uid="{90ACD433-CF4C-4370-B351-0D97CA1A2189}" name="Day"/>
-    <tableColumn id="9" xr3:uid="{BBED0197-BB85-4165-A816-02E8E2B7B387}" name="Best Lap Time" dataDxfId="1">
+    <tableColumn id="9" xr3:uid="{BBED0197-BB85-4165-A816-02E8E2B7B387}" name="Best Lap Time" dataDxfId="2">
       <calculatedColumnFormula>SUBSTITUTE(D2, "s", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{7B18573B-AA06-4662-B8EE-F205A25E907B}" name="Gap to Best Lap Time" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{7B18573B-AA06-4662-B8EE-F205A25E907B}" name="Gap to Best Lap Time" dataDxfId="1">
       <calculatedColumnFormula>SUBSTITUTE(SUBSTITUTE(E2,"+",""), "s", "")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{131BADD9-CF56-407E-902D-8AC6BAD64AAD}" name="Best Lap Times" dataDxfId="0">
+      <calculatedColumnFormula>SUBSTITUTE(SUBSTITUTE(D2,":",""), "s", "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2402,10 +2411,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85BF523-30CB-48A7-8E76-D50239268866}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2416,10 +2425,10 @@
     <col min="4" max="4" width="12.5546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="4" customWidth="1"/>
     <col min="10" max="10" width="20.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>151</v>
       </c>
@@ -2450,8 +2459,11 @@
       <c r="J1" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2484,8 +2496,12 @@
         <f>SUBSTITUTE(SUBSTITUTE(E2,"+",""), "s", "")</f>
         <v>0.000</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" s="1" t="str">
+        <f t="shared" ref="K2:K33" si="1">SUBSTITUTE(SUBSTITUTE(D2,":",""), "s", "")</f>
+        <v>131.344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2515,11 +2531,15 @@
         <v>1:32.484</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f t="shared" ref="J3:J19" si="1">SUBSTITUTE(SUBSTITUTE(E3,"+",""), "s", "")</f>
+        <f t="shared" ref="J3:J19" si="2">SUBSTITUTE(SUBSTITUTE(E3,"+",""), "s", "")</f>
         <v>1.140</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>132.484</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2549,11 +2569,15 @@
         <v>1:32.584</v>
       </c>
       <c r="J4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1.240</v>
+      </c>
+      <c r="K4" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>1.240</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>132.584</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2583,11 +2607,15 @@
         <v>1:32.599</v>
       </c>
       <c r="J5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1.255</v>
+      </c>
+      <c r="K5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>1.255</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>132.599</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2617,11 +2645,15 @@
         <v>1:32.805</v>
       </c>
       <c r="J6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1.461</v>
+      </c>
+      <c r="K6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>1.461</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>132.805</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2651,11 +2683,15 @@
         <v>1:33.007</v>
       </c>
       <c r="J7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1.663</v>
+      </c>
+      <c r="K7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>1.663</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>133.007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2685,11 +2721,15 @@
         <v>1:33.247</v>
       </c>
       <c r="J8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1.903</v>
+      </c>
+      <c r="K8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>1.903</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>133.247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2719,11 +2759,15 @@
         <v>1:33.385</v>
       </c>
       <c r="J9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>2.041</v>
+      </c>
+      <c r="K9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>2.041</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>133.385</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2753,11 +2797,15 @@
         <v>1:33.658</v>
       </c>
       <c r="J10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>2.314</v>
+      </c>
+      <c r="K10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>2.314</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>133.658</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2787,11 +2835,15 @@
         <v>1:33.871</v>
       </c>
       <c r="J11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>2.527</v>
+      </c>
+      <c r="K11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>2.527</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>133.871</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2821,11 +2873,15 @@
         <v>1:33.882</v>
       </c>
       <c r="J12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>2.538</v>
+      </c>
+      <c r="K12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>2.538</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>133.882</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2855,11 +2911,15 @@
         <v>1:34.109</v>
       </c>
       <c r="J13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>2.765</v>
+      </c>
+      <c r="K13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>2.765</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>134.109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2889,11 +2949,15 @@
         <v>1:34.136</v>
       </c>
       <c r="J14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>2.792</v>
+      </c>
+      <c r="K14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>2.792</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>134.136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2923,11 +2987,15 @@
         <v>1:34.431</v>
       </c>
       <c r="J15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>3.087</v>
+      </c>
+      <c r="K15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>3.087</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>134.431</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2957,11 +3025,15 @@
         <v>1:34.587</v>
       </c>
       <c r="J16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>3.243</v>
+      </c>
+      <c r="K16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>3.243</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+        <v>134.587</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2991,11 +3063,15 @@
         <v>1:34.677</v>
       </c>
       <c r="J17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>3.333</v>
+      </c>
+      <c r="K17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>3.333</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+        <v>134.677</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3025,11 +3101,15 @@
         <v>1:35.692</v>
       </c>
       <c r="J18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>4.348</v>
+      </c>
+      <c r="K18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>4.348</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+        <v>135.692</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3059,11 +3139,15 @@
         <v>1:35.906</v>
       </c>
       <c r="J19" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>4.562</v>
+      </c>
+      <c r="K19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>4.562</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+        <v>135.906</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -3096,8 +3180,12 @@
         <f>SUBSTITUTE(SUBSTITUTE(E20,"+",""), "s", "")</f>
         <v>0.000</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>129.921</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3123,15 +3211,19 @@
         <v>2</v>
       </c>
       <c r="I21" s="4" t="str">
-        <f t="shared" ref="I21:I36" si="2">SUBSTITUTE(D21, "s", "")</f>
+        <f t="shared" ref="I21:I36" si="3">SUBSTITUTE(D21, "s", "")</f>
         <v>1:30.679</v>
       </c>
       <c r="J21" s="1" t="str">
-        <f t="shared" ref="J21:J36" si="3">SUBSTITUTE(SUBSTITUTE(E21,"+",""), "s", "")</f>
+        <f t="shared" ref="J21:J36" si="4">SUBSTITUTE(SUBSTITUTE(E21,"+",""), "s", "")</f>
         <v>0.758</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>130.679</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -3157,15 +3249,19 @@
         <v>2</v>
       </c>
       <c r="I22" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:31.066</v>
       </c>
       <c r="J22" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.145</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>131.066</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4</v>
       </c>
@@ -3191,15 +3287,19 @@
         <v>2</v>
       </c>
       <c r="I23" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:31.256</v>
       </c>
       <c r="J23" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.335</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>131.256</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -3225,15 +3325,19 @@
         <v>2</v>
       </c>
       <c r="I24" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:31.361</v>
       </c>
       <c r="J24" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.440</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>131.361</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>6</v>
       </c>
@@ -3259,15 +3363,19 @@
         <v>2</v>
       </c>
       <c r="I25" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:31.750</v>
       </c>
       <c r="J25" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.829</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>131.750</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>7</v>
       </c>
@@ -3293,15 +3401,19 @@
         <v>2</v>
       </c>
       <c r="I26" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:32.029</v>
       </c>
       <c r="J26" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.108</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>132.029</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8</v>
       </c>
@@ -3327,15 +3439,19 @@
         <v>2</v>
       </c>
       <c r="I27" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:32.061</v>
       </c>
       <c r="J27" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.140</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>132.061</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>9</v>
       </c>
@@ -3361,15 +3477,19 @@
         <v>2</v>
       </c>
       <c r="I28" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:32.227</v>
       </c>
       <c r="J28" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.306</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>132.227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10</v>
       </c>
@@ -3395,15 +3515,19 @@
         <v>2</v>
       </c>
       <c r="I29" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:32.328</v>
       </c>
       <c r="J29" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.407</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>132.328</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>11</v>
       </c>
@@ -3429,15 +3553,19 @@
         <v>2</v>
       </c>
       <c r="I30" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:32.578</v>
       </c>
       <c r="J30" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.657</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K30" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>132.578</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>12</v>
       </c>
@@ -3463,15 +3591,19 @@
         <v>2</v>
       </c>
       <c r="I31" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:33.053</v>
       </c>
       <c r="J31" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.132</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>133.053</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>13</v>
       </c>
@@ -3497,15 +3629,19 @@
         <v>2</v>
       </c>
       <c r="I32" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:33.715</v>
       </c>
       <c r="J32" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.794</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K32" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>133.715</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>14</v>
       </c>
@@ -3531,15 +3667,19 @@
         <v>2</v>
       </c>
       <c r="I33" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:33.804</v>
       </c>
       <c r="J33" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.883</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K33" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>133.804</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>15</v>
       </c>
@@ -3565,15 +3705,19 @@
         <v>2</v>
       </c>
       <c r="I34" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:36.611</v>
       </c>
       <c r="J34" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.690</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K34" s="1" t="str">
+        <f t="shared" ref="K34:K55" si="5">SUBSTITUTE(SUBSTITUTE(D34,":",""), "s", "")</f>
+        <v>136.611</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>16</v>
       </c>
@@ -3599,15 +3743,19 @@
         <v>2</v>
       </c>
       <c r="I35" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:37.509</v>
       </c>
       <c r="J35" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.588</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K35" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>137.509</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>17</v>
       </c>
@@ -3633,15 +3781,19 @@
         <v>2</v>
       </c>
       <c r="I36" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1:38.074</v>
       </c>
       <c r="J36" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.153</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K36" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>138.074</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
@@ -3667,15 +3819,19 @@
         <v>3</v>
       </c>
       <c r="I37" s="4" t="str">
-        <f t="shared" ref="I37:I55" si="4">SUBSTITUTE(D37, "s", "")</f>
+        <f t="shared" ref="I37:I55" si="6">SUBSTITUTE(D37, "s", "")</f>
         <v>1:30.322</v>
       </c>
       <c r="J37" s="1" t="str">
-        <f t="shared" ref="J37:J55" si="5">SUBSTITUTE(SUBSTITUTE(E37,"+",""), "s", "")</f>
+        <f t="shared" ref="J37:J55" si="7">SUBSTITUTE(SUBSTITUTE(E37,"+",""), "s", "")</f>
         <v>0.000</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K37" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>130.322</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2</v>
       </c>
@@ -3701,15 +3857,19 @@
         <v>3</v>
       </c>
       <c r="I38" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:30.368</v>
       </c>
       <c r="J38" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>0.046</v>
+      </c>
+      <c r="K38" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>0.046</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+        <v>130.368</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3</v>
       </c>
@@ -3735,15 +3895,19 @@
         <v>3</v>
       </c>
       <c r="I39" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:30.647</v>
       </c>
       <c r="J39" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>0.325</v>
+      </c>
+      <c r="K39" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+        <v>130.647</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3769,15 +3933,19 @@
         <v>3</v>
       </c>
       <c r="I40" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:30.755</v>
       </c>
       <c r="J40" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>0.433</v>
+      </c>
+      <c r="K40" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>0.433</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+        <v>130.755</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>5</v>
       </c>
@@ -3803,15 +3971,19 @@
         <v>3</v>
       </c>
       <c r="I41" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:30.775</v>
       </c>
       <c r="J41" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>0.453</v>
+      </c>
+      <c r="K41" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>0.453</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+        <v>130.775</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>6</v>
       </c>
@@ -3837,15 +4009,19 @@
         <v>3</v>
       </c>
       <c r="I42" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:30.984</v>
       </c>
       <c r="J42" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>0.662</v>
+      </c>
+      <c r="K42" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>0.662</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+        <v>130.984</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>7</v>
       </c>
@@ -3871,15 +4047,19 @@
         <v>3</v>
       </c>
       <c r="I43" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:31.030</v>
       </c>
       <c r="J43" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>0.708</v>
+      </c>
+      <c r="K43" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>0.708</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+        <v>131.030</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>8</v>
       </c>
@@ -3905,15 +4085,19 @@
         <v>3</v>
       </c>
       <c r="I44" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:31.159</v>
       </c>
       <c r="J44" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>0.837</v>
+      </c>
+      <c r="K44" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>0.837</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+        <v>131.159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>9</v>
       </c>
@@ -3939,15 +4123,19 @@
         <v>3</v>
       </c>
       <c r="I45" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:31.247</v>
       </c>
       <c r="J45" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>0.925</v>
+      </c>
+      <c r="K45" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>0.925</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+        <v>131.247</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>10</v>
       </c>
@@ -3973,15 +4161,19 @@
         <v>3</v>
       </c>
       <c r="I46" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:31.483</v>
       </c>
       <c r="J46" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>1.161</v>
+      </c>
+      <c r="K46" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>1.161</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+        <v>131.483</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>11</v>
       </c>
@@ -4007,15 +4199,19 @@
         <v>3</v>
       </c>
       <c r="I47" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:31.686</v>
       </c>
       <c r="J47" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>1.364</v>
+      </c>
+      <c r="K47" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>1.364</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+        <v>131.686</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>12</v>
       </c>
@@ -4041,15 +4237,19 @@
         <v>3</v>
       </c>
       <c r="I48" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:31.999</v>
       </c>
       <c r="J48" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>1.677</v>
+      </c>
+      <c r="K48" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>1.677</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+        <v>131.999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>13</v>
       </c>
@@ -4075,15 +4275,19 @@
         <v>3</v>
       </c>
       <c r="I49" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:32.038</v>
       </c>
       <c r="J49" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>1.716</v>
+      </c>
+      <c r="K49" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>1.716</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+        <v>132.038</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>14</v>
       </c>
@@ -4109,15 +4313,19 @@
         <v>3</v>
       </c>
       <c r="I50" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:32.108</v>
       </c>
       <c r="J50" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>1.786</v>
+      </c>
+      <c r="K50" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>1.786</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+        <v>132.108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>15</v>
       </c>
@@ -4143,15 +4351,19 @@
         <v>3</v>
       </c>
       <c r="I51" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:32.149</v>
       </c>
       <c r="J51" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>1.827</v>
+      </c>
+      <c r="K51" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>1.827</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+        <v>132.149</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>16</v>
       </c>
@@ -4177,15 +4389,19 @@
         <v>3</v>
       </c>
       <c r="I52" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:33.053</v>
       </c>
       <c r="J52" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>2.731</v>
+      </c>
+      <c r="K52" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>2.731</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+        <v>133.053</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>17</v>
       </c>
@@ -4211,15 +4427,19 @@
         <v>3</v>
       </c>
       <c r="I53" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:33.079</v>
       </c>
       <c r="J53" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>2.757</v>
+      </c>
+      <c r="K53" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>2.757</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+        <v>133.079</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>18</v>
       </c>
@@ -4245,15 +4465,19 @@
         <v>3</v>
       </c>
       <c r="I54" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:33.528</v>
       </c>
       <c r="J54" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>3.206</v>
+      </c>
+      <c r="K54" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>3.206</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+        <v>133.528</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>19</v>
       </c>
@@ -4279,12 +4503,16 @@
         <v>3</v>
       </c>
       <c r="I55" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1:37.015</v>
       </c>
       <c r="J55" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>6.693</v>
+      </c>
+      <c r="K55" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>6.693</v>
+        <v>137.015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>